<commit_message>
Migrate e2e mock flow without api calls from flask to hapi
</commit_message>
<xml_diff>
--- a/tool/test-packs/homecare_all_types.xlsx
+++ b/tool/test-packs/homecare_all_types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e\tool\test-packs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6186D23-78C7-4ABC-9ABF-7A24FC314275}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68F45B69-1A80-4B68-B647-8F920BD3330F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="2" xr2:uid="{7C3F71BD-1F0F-4548-8705-713F65ABAC71}"/>
   </bookViews>
@@ -3886,7 +3886,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Fix test-pack sending for examples in repo
</commit_message>
<xml_diff>
--- a/tool/test-packs/homecare_all_types.xlsx
+++ b/tool/test-packs/homecare_all_types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e\tool\test-packs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68F45B69-1A80-4B68-B647-8F920BD3330F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F2C243-22A1-4DAE-B446-D7AC16AC4C08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="2" xr2:uid="{7C3F71BD-1F0F-4548-8705-713F65ABAC71}"/>
   </bookViews>
@@ -3886,7 +3886,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
AEA-1837: Fix test-pack send prescription user-journey for examples in repo (#644)
* Fix test-pack sending for examples in repo

* PR feedback

* Update send component load messaging to show it can be one or more prescriptions

* Fix copy button for send bulk result
</commit_message>
<xml_diff>
--- a/tool/test-packs/homecare_all_types.xlsx
+++ b/tool/test-packs/homecare_all_types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e\tool\test-packs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68F45B69-1A80-4B68-B647-8F920BD3330F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F2C243-22A1-4DAE-B446-D7AC16AC4C08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="2" xr2:uid="{7C3F71BD-1F0F-4548-8705-713F65ABAC71}"/>
   </bookViews>
@@ -3886,7 +3886,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
AEA-1822: Merge in other PR branch. Update type guards for send operation.
</commit_message>
<xml_diff>
--- a/tool/test-packs/homecare_all_types.xlsx
+++ b/tool/test-packs/homecare_all_types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e\tool\test-packs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68F45B69-1A80-4B68-B647-8F920BD3330F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F2C243-22A1-4DAE-B446-D7AC16AC4C08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="2" xr2:uid="{7C3F71BD-1F0F-4548-8705-713F65ABAC71}"/>
   </bookViews>
@@ -3886,7 +3886,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>